<commit_message>
Tri Truong _ Note
</commit_message>
<xml_diff>
--- a/01_Document/TM_Design_v1.0.xlsx
+++ b/01_Document/TM_Design_v1.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Document\TimMart\TimMart\01_Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NTP\TimMart\01_Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" tabRatio="880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" tabRatio="880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MoDau" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="104">
   <si>
     <t>Người tạo</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>CODING</t>
+  </si>
+  <si>
+    <t>TriTruong</t>
+  </si>
+  <si>
+    <t>Note: Cấu trúc tên biến" tenmota_Chucnang ", tên hàm "tenmota_Chucnang" . Ex: (username_ad &amp; username ...) . (getInfo_user &amp; getInfo_ad) ….</t>
   </si>
 </sst>
 </file>
@@ -816,9 +822,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -826,6 +829,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -837,40 +876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1375,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3394,8 +3400,8 @@
   <dimension ref="A1:AV21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3912,9 +3918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:AV3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4038,633 +4044,685 @@
       <c r="AU2" s="33"/>
       <c r="AV2" s="34"/>
     </row>
+    <row r="3" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64"/>
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+      <c r="AV3" s="64"/>
+    </row>
     <row r="4" spans="1:48" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="58" t="s">
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="58" t="s">
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="59"/>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="60"/>
-      <c r="AC4" s="58" t="s">
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="55"/>
+      <c r="AC4" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59"/>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59"/>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="59"/>
-      <c r="AL4" s="59"/>
-      <c r="AM4" s="59"/>
-      <c r="AN4" s="59"/>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="60"/>
-      <c r="AQ4" s="58" t="s">
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="54"/>
+      <c r="AF4" s="54"/>
+      <c r="AG4" s="54"/>
+      <c r="AH4" s="54"/>
+      <c r="AI4" s="54"/>
+      <c r="AJ4" s="54"/>
+      <c r="AK4" s="54"/>
+      <c r="AL4" s="54"/>
+      <c r="AM4" s="54"/>
+      <c r="AN4" s="54"/>
+      <c r="AO4" s="54"/>
+      <c r="AP4" s="55"/>
+      <c r="AQ4" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="AR4" s="59"/>
-      <c r="AS4" s="59"/>
-      <c r="AT4" s="60"/>
-      <c r="AU4" s="58" t="s">
+      <c r="AR4" s="54"/>
+      <c r="AS4" s="54"/>
+      <c r="AT4" s="55"/>
+      <c r="AU4" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="AV4" s="60"/>
+      <c r="AV4" s="55"/>
     </row>
     <row r="5" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="49" t="s">
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="52" t="s">
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
-      <c r="W5" s="53"/>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="53"/>
-      <c r="Z5" s="53"/>
-      <c r="AA5" s="53"/>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="55" t="s">
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="64"/>
+      <c r="S5" s="64"/>
+      <c r="T5" s="64"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64"/>
+      <c r="W5" s="64"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="64"/>
+      <c r="Z5" s="64"/>
+      <c r="AA5" s="64"/>
+      <c r="AB5" s="65"/>
+      <c r="AC5" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="AD5" s="56"/>
-      <c r="AE5" s="56"/>
-      <c r="AF5" s="56"/>
-      <c r="AG5" s="56"/>
-      <c r="AH5" s="56"/>
-      <c r="AI5" s="56"/>
-      <c r="AJ5" s="56"/>
-      <c r="AK5" s="56"/>
-      <c r="AL5" s="56"/>
-      <c r="AM5" s="56"/>
-      <c r="AN5" s="56"/>
-      <c r="AO5" s="56"/>
-      <c r="AP5" s="57"/>
-      <c r="AQ5" s="49" t="s">
+      <c r="AD5" s="57"/>
+      <c r="AE5" s="57"/>
+      <c r="AF5" s="57"/>
+      <c r="AG5" s="57"/>
+      <c r="AH5" s="57"/>
+      <c r="AI5" s="57"/>
+      <c r="AJ5" s="57"/>
+      <c r="AK5" s="57"/>
+      <c r="AL5" s="57"/>
+      <c r="AM5" s="57"/>
+      <c r="AN5" s="57"/>
+      <c r="AO5" s="57"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AR5" s="50"/>
-      <c r="AS5" s="50"/>
-      <c r="AT5" s="51"/>
-      <c r="AU5" s="65" t="s">
+      <c r="AR5" s="49"/>
+      <c r="AS5" s="49"/>
+      <c r="AT5" s="50"/>
+      <c r="AU5" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="AV5" s="66"/>
+      <c r="AV5" s="52"/>
     </row>
     <row r="6" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <f>MAX($A5)+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="49" t="s">
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="52" t="s">
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="53"/>
-      <c r="Y6" s="53"/>
-      <c r="Z6" s="53"/>
-      <c r="AA6" s="53"/>
-      <c r="AB6" s="54"/>
-      <c r="AC6" s="55" t="s">
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
+      <c r="Q6" s="64"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="64"/>
+      <c r="T6" s="64"/>
+      <c r="U6" s="64"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="64"/>
+      <c r="X6" s="64"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="64"/>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="65"/>
+      <c r="AC6" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="AD6" s="56"/>
-      <c r="AE6" s="56"/>
-      <c r="AF6" s="56"/>
-      <c r="AG6" s="56"/>
-      <c r="AH6" s="56"/>
-      <c r="AI6" s="56"/>
-      <c r="AJ6" s="56"/>
-      <c r="AK6" s="56"/>
-      <c r="AL6" s="56"/>
-      <c r="AM6" s="56"/>
-      <c r="AN6" s="56"/>
-      <c r="AO6" s="56"/>
-      <c r="AP6" s="57"/>
-      <c r="AQ6" s="49" t="s">
+      <c r="AD6" s="57"/>
+      <c r="AE6" s="57"/>
+      <c r="AF6" s="57"/>
+      <c r="AG6" s="57"/>
+      <c r="AH6" s="57"/>
+      <c r="AI6" s="57"/>
+      <c r="AJ6" s="57"/>
+      <c r="AK6" s="57"/>
+      <c r="AL6" s="57"/>
+      <c r="AM6" s="57"/>
+      <c r="AN6" s="57"/>
+      <c r="AO6" s="57"/>
+      <c r="AP6" s="58"/>
+      <c r="AQ6" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="AR6" s="50"/>
-      <c r="AS6" s="50"/>
-      <c r="AT6" s="51"/>
-      <c r="AU6" s="65" t="s">
+      <c r="AR6" s="49"/>
+      <c r="AS6" s="49"/>
+      <c r="AT6" s="50"/>
+      <c r="AU6" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="AV6" s="66"/>
+      <c r="AV6" s="52"/>
     </row>
     <row r="7" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <f t="shared" ref="A7:A21" si="0">MAX($A6)+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="49" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="52" t="s">
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="53"/>
-      <c r="Y7" s="53"/>
-      <c r="Z7" s="53"/>
-      <c r="AA7" s="53"/>
-      <c r="AB7" s="54"/>
-      <c r="AC7" s="55" t="s">
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="64"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="64"/>
+      <c r="U7" s="64"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="64"/>
+      <c r="X7" s="64"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
+      <c r="AA7" s="64"/>
+      <c r="AB7" s="65"/>
+      <c r="AC7" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="AD7" s="56"/>
-      <c r="AE7" s="56"/>
-      <c r="AF7" s="56"/>
-      <c r="AG7" s="56"/>
-      <c r="AH7" s="56"/>
-      <c r="AI7" s="56"/>
-      <c r="AJ7" s="56"/>
-      <c r="AK7" s="56"/>
-      <c r="AL7" s="56"/>
-      <c r="AM7" s="56"/>
-      <c r="AN7" s="56"/>
-      <c r="AO7" s="56"/>
-      <c r="AP7" s="57"/>
-      <c r="AQ7" s="49" t="s">
+      <c r="AD7" s="57"/>
+      <c r="AE7" s="57"/>
+      <c r="AF7" s="57"/>
+      <c r="AG7" s="57"/>
+      <c r="AH7" s="57"/>
+      <c r="AI7" s="57"/>
+      <c r="AJ7" s="57"/>
+      <c r="AK7" s="57"/>
+      <c r="AL7" s="57"/>
+      <c r="AM7" s="57"/>
+      <c r="AN7" s="57"/>
+      <c r="AO7" s="57"/>
+      <c r="AP7" s="58"/>
+      <c r="AQ7" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="AR7" s="50"/>
-      <c r="AS7" s="50"/>
-      <c r="AT7" s="51"/>
-      <c r="AU7" s="65" t="s">
+      <c r="AR7" s="49"/>
+      <c r="AS7" s="49"/>
+      <c r="AT7" s="50"/>
+      <c r="AU7" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="AV7" s="66"/>
+      <c r="AV7" s="52"/>
     </row>
     <row r="8" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="49" t="s">
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="48" t="s">
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="48"/>
-      <c r="X8" s="48"/>
-      <c r="Y8" s="48"/>
-      <c r="Z8" s="48"/>
-      <c r="AA8" s="48"/>
-      <c r="AB8" s="48"/>
-      <c r="AC8" s="55" t="s">
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+      <c r="S8" s="61"/>
+      <c r="T8" s="61"/>
+      <c r="U8" s="61"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="61"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="61"/>
+      <c r="Z8" s="61"/>
+      <c r="AA8" s="61"/>
+      <c r="AB8" s="61"/>
+      <c r="AC8" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="AD8" s="56"/>
-      <c r="AE8" s="56"/>
-      <c r="AF8" s="56"/>
-      <c r="AG8" s="56"/>
-      <c r="AH8" s="56"/>
-      <c r="AI8" s="56"/>
-      <c r="AJ8" s="56"/>
-      <c r="AK8" s="56"/>
-      <c r="AL8" s="56"/>
-      <c r="AM8" s="56"/>
-      <c r="AN8" s="56"/>
-      <c r="AO8" s="56"/>
-      <c r="AP8" s="57"/>
-      <c r="AQ8" s="49" t="s">
+      <c r="AD8" s="57"/>
+      <c r="AE8" s="57"/>
+      <c r="AF8" s="57"/>
+      <c r="AG8" s="57"/>
+      <c r="AH8" s="57"/>
+      <c r="AI8" s="57"/>
+      <c r="AJ8" s="57"/>
+      <c r="AK8" s="57"/>
+      <c r="AL8" s="57"/>
+      <c r="AM8" s="57"/>
+      <c r="AN8" s="57"/>
+      <c r="AO8" s="57"/>
+      <c r="AP8" s="58"/>
+      <c r="AQ8" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="50"/>
-      <c r="AS8" s="50"/>
-      <c r="AT8" s="51"/>
-      <c r="AU8" s="65" t="s">
+      <c r="AR8" s="49"/>
+      <c r="AS8" s="49"/>
+      <c r="AT8" s="50"/>
+      <c r="AU8" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="AV8" s="66"/>
+      <c r="AV8" s="52"/>
     </row>
     <row r="9" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="49" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="48" t="s">
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="48"/>
-      <c r="U9" s="48"/>
-      <c r="V9" s="48"/>
-      <c r="W9" s="48"/>
-      <c r="X9" s="48"/>
-      <c r="Y9" s="48"/>
-      <c r="Z9" s="48"/>
-      <c r="AA9" s="48"/>
-      <c r="AB9" s="48"/>
-      <c r="AC9" s="55" t="s">
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="61"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="61"/>
+      <c r="AB9" s="61"/>
+      <c r="AC9" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="AD9" s="56"/>
-      <c r="AE9" s="56"/>
-      <c r="AF9" s="56"/>
-      <c r="AG9" s="56"/>
-      <c r="AH9" s="56"/>
-      <c r="AI9" s="56"/>
-      <c r="AJ9" s="56"/>
-      <c r="AK9" s="56"/>
-      <c r="AL9" s="56"/>
-      <c r="AM9" s="56"/>
-      <c r="AN9" s="56"/>
-      <c r="AO9" s="56"/>
-      <c r="AP9" s="57"/>
-      <c r="AQ9" s="49" t="s">
+      <c r="AD9" s="57"/>
+      <c r="AE9" s="57"/>
+      <c r="AF9" s="57"/>
+      <c r="AG9" s="57"/>
+      <c r="AH9" s="57"/>
+      <c r="AI9" s="57"/>
+      <c r="AJ9" s="57"/>
+      <c r="AK9" s="57"/>
+      <c r="AL9" s="57"/>
+      <c r="AM9" s="57"/>
+      <c r="AN9" s="57"/>
+      <c r="AO9" s="57"/>
+      <c r="AP9" s="58"/>
+      <c r="AQ9" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AR9" s="50"/>
-      <c r="AS9" s="50"/>
-      <c r="AT9" s="51"/>
-      <c r="AU9" s="65" t="s">
+      <c r="AR9" s="49"/>
+      <c r="AS9" s="49"/>
+      <c r="AT9" s="50"/>
+      <c r="AU9" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="AV9" s="66"/>
+      <c r="AV9" s="52"/>
     </row>
     <row r="10" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="49" t="s">
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="48" t="s">
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="48"/>
-      <c r="U10" s="48"/>
-      <c r="V10" s="48"/>
-      <c r="W10" s="48"/>
-      <c r="X10" s="48"/>
-      <c r="Y10" s="48"/>
-      <c r="Z10" s="48"/>
-      <c r="AA10" s="48"/>
-      <c r="AB10" s="48"/>
-      <c r="AC10" s="55" t="s">
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="61"/>
+      <c r="R10" s="61"/>
+      <c r="S10" s="61"/>
+      <c r="T10" s="61"/>
+      <c r="U10" s="61"/>
+      <c r="V10" s="61"/>
+      <c r="W10" s="61"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="61"/>
+      <c r="Z10" s="61"/>
+      <c r="AA10" s="61"/>
+      <c r="AB10" s="61"/>
+      <c r="AC10" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="AD10" s="56"/>
-      <c r="AE10" s="56"/>
-      <c r="AF10" s="56"/>
-      <c r="AG10" s="56"/>
-      <c r="AH10" s="56"/>
-      <c r="AI10" s="56"/>
-      <c r="AJ10" s="56"/>
-      <c r="AK10" s="56"/>
-      <c r="AL10" s="56"/>
-      <c r="AM10" s="56"/>
-      <c r="AN10" s="56"/>
-      <c r="AO10" s="56"/>
-      <c r="AP10" s="57"/>
-      <c r="AQ10" s="49" t="s">
+      <c r="AD10" s="57"/>
+      <c r="AE10" s="57"/>
+      <c r="AF10" s="57"/>
+      <c r="AG10" s="57"/>
+      <c r="AH10" s="57"/>
+      <c r="AI10" s="57"/>
+      <c r="AJ10" s="57"/>
+      <c r="AK10" s="57"/>
+      <c r="AL10" s="57"/>
+      <c r="AM10" s="57"/>
+      <c r="AN10" s="57"/>
+      <c r="AO10" s="57"/>
+      <c r="AP10" s="58"/>
+      <c r="AQ10" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="AR10" s="50"/>
-      <c r="AS10" s="50"/>
-      <c r="AT10" s="51"/>
-      <c r="AU10" s="65" t="s">
+      <c r="AR10" s="49"/>
+      <c r="AS10" s="49"/>
+      <c r="AT10" s="50"/>
+      <c r="AU10" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="AV10" s="66"/>
+      <c r="AV10" s="52"/>
     </row>
     <row r="11" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="49" t="s">
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="48" t="s">
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="48"/>
-      <c r="Z11" s="48"/>
-      <c r="AA11" s="48"/>
-      <c r="AB11" s="48"/>
-      <c r="AC11" s="63" t="s">
+      <c r="N11" s="61"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="61"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="61"/>
+      <c r="U11" s="61"/>
+      <c r="V11" s="61"/>
+      <c r="W11" s="61"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="61"/>
+      <c r="Z11" s="61"/>
+      <c r="AA11" s="61"/>
+      <c r="AB11" s="61"/>
+      <c r="AC11" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="AD11" s="63"/>
-      <c r="AE11" s="63"/>
-      <c r="AF11" s="63"/>
-      <c r="AG11" s="63"/>
-      <c r="AH11" s="63"/>
-      <c r="AI11" s="63"/>
-      <c r="AJ11" s="63"/>
-      <c r="AK11" s="63"/>
-      <c r="AL11" s="63"/>
-      <c r="AM11" s="63"/>
-      <c r="AN11" s="63"/>
-      <c r="AO11" s="63"/>
-      <c r="AP11" s="63"/>
-      <c r="AQ11" s="49" t="s">
+      <c r="AD11" s="59"/>
+      <c r="AE11" s="59"/>
+      <c r="AF11" s="59"/>
+      <c r="AG11" s="59"/>
+      <c r="AH11" s="59"/>
+      <c r="AI11" s="59"/>
+      <c r="AJ11" s="59"/>
+      <c r="AK11" s="59"/>
+      <c r="AL11" s="59"/>
+      <c r="AM11" s="59"/>
+      <c r="AN11" s="59"/>
+      <c r="AO11" s="59"/>
+      <c r="AP11" s="59"/>
+      <c r="AQ11" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="AR11" s="50"/>
-      <c r="AS11" s="50"/>
-      <c r="AT11" s="51"/>
-      <c r="AU11" s="65" t="s">
+      <c r="AR11" s="49"/>
+      <c r="AS11" s="49"/>
+      <c r="AT11" s="50"/>
+      <c r="AU11" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="AV11" s="66"/>
+      <c r="AV11" s="52"/>
     </row>
     <row r="12" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="49" t="s">
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="48" t="s">
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="48"/>
-      <c r="Y12" s="48"/>
-      <c r="Z12" s="48"/>
-      <c r="AA12" s="48"/>
-      <c r="AB12" s="48"/>
-      <c r="AC12" s="64" t="s">
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="61"/>
+      <c r="U12" s="61"/>
+      <c r="V12" s="61"/>
+      <c r="W12" s="61"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="61"/>
+      <c r="Z12" s="61"/>
+      <c r="AA12" s="61"/>
+      <c r="AB12" s="61"/>
+      <c r="AC12" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="AD12" s="64"/>
-      <c r="AE12" s="64"/>
-      <c r="AF12" s="64"/>
-      <c r="AG12" s="64"/>
-      <c r="AH12" s="64"/>
-      <c r="AI12" s="64"/>
-      <c r="AJ12" s="64"/>
-      <c r="AK12" s="64"/>
-      <c r="AL12" s="64"/>
-      <c r="AM12" s="64"/>
-      <c r="AN12" s="64"/>
-      <c r="AO12" s="64"/>
-      <c r="AP12" s="64"/>
-      <c r="AQ12" s="49" t="s">
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="60"/>
+      <c r="AH12" s="60"/>
+      <c r="AI12" s="60"/>
+      <c r="AJ12" s="60"/>
+      <c r="AK12" s="60"/>
+      <c r="AL12" s="60"/>
+      <c r="AM12" s="60"/>
+      <c r="AN12" s="60"/>
+      <c r="AO12" s="60"/>
+      <c r="AP12" s="60"/>
+      <c r="AQ12" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AR12" s="50"/>
-      <c r="AS12" s="50"/>
-      <c r="AT12" s="51"/>
-      <c r="AU12" s="65"/>
-      <c r="AV12" s="66"/>
+      <c r="AR12" s="49"/>
+      <c r="AS12" s="49"/>
+      <c r="AT12" s="50"/>
+      <c r="AU12" s="51"/>
+      <c r="AV12" s="52"/>
     </row>
     <row r="13" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="49" t="s">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="48" t="s">
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
-      <c r="X13" s="48"/>
-      <c r="Y13" s="48"/>
-      <c r="Z13" s="48"/>
-      <c r="AA13" s="48"/>
-      <c r="AB13" s="48"/>
-      <c r="AC13" s="64" t="s">
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="61"/>
+      <c r="S13" s="61"/>
+      <c r="T13" s="61"/>
+      <c r="U13" s="61"/>
+      <c r="V13" s="61"/>
+      <c r="W13" s="61"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="61"/>
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="61"/>
+      <c r="AC13" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="AD13" s="64"/>
-      <c r="AE13" s="64"/>
-      <c r="AF13" s="64"/>
-      <c r="AG13" s="64"/>
-      <c r="AH13" s="64"/>
-      <c r="AI13" s="64"/>
-      <c r="AJ13" s="64"/>
-      <c r="AK13" s="64"/>
-      <c r="AL13" s="64"/>
-      <c r="AM13" s="64"/>
-      <c r="AN13" s="64"/>
-      <c r="AO13" s="64"/>
-      <c r="AP13" s="64"/>
-      <c r="AQ13" s="49" t="s">
+      <c r="AD13" s="60"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="60"/>
+      <c r="AG13" s="60"/>
+      <c r="AH13" s="60"/>
+      <c r="AI13" s="60"/>
+      <c r="AJ13" s="60"/>
+      <c r="AK13" s="60"/>
+      <c r="AL13" s="60"/>
+      <c r="AM13" s="60"/>
+      <c r="AN13" s="60"/>
+      <c r="AO13" s="60"/>
+      <c r="AP13" s="60"/>
+      <c r="AQ13" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AR13" s="50"/>
-      <c r="AS13" s="50"/>
-      <c r="AT13" s="51"/>
-      <c r="AU13" s="65"/>
-      <c r="AV13" s="66"/>
+      <c r="AR13" s="49"/>
+      <c r="AS13" s="49"/>
+      <c r="AT13" s="50"/>
+      <c r="AU13" s="51"/>
+      <c r="AV13" s="52"/>
     </row>
     <row r="14" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -4680,54 +4738,54 @@
       <c r="F14" s="62"/>
       <c r="G14" s="62"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="49" t="s">
+      <c r="I14" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="48" t="s">
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
-      <c r="X14" s="48"/>
-      <c r="Y14" s="48"/>
-      <c r="Z14" s="48"/>
-      <c r="AA14" s="48"/>
-      <c r="AB14" s="48"/>
-      <c r="AC14" s="64" t="s">
+      <c r="N14" s="61"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="61"/>
+      <c r="T14" s="61"/>
+      <c r="U14" s="61"/>
+      <c r="V14" s="61"/>
+      <c r="W14" s="61"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="61"/>
+      <c r="Z14" s="61"/>
+      <c r="AA14" s="61"/>
+      <c r="AB14" s="61"/>
+      <c r="AC14" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="AD14" s="64"/>
-      <c r="AE14" s="64"/>
-      <c r="AF14" s="64"/>
-      <c r="AG14" s="64"/>
-      <c r="AH14" s="64"/>
-      <c r="AI14" s="64"/>
-      <c r="AJ14" s="64"/>
-      <c r="AK14" s="64"/>
-      <c r="AL14" s="64"/>
-      <c r="AM14" s="64"/>
-      <c r="AN14" s="64"/>
-      <c r="AO14" s="64"/>
-      <c r="AP14" s="64"/>
-      <c r="AQ14" s="49" t="s">
+      <c r="AD14" s="60"/>
+      <c r="AE14" s="60"/>
+      <c r="AF14" s="60"/>
+      <c r="AG14" s="60"/>
+      <c r="AH14" s="60"/>
+      <c r="AI14" s="60"/>
+      <c r="AJ14" s="60"/>
+      <c r="AK14" s="60"/>
+      <c r="AL14" s="60"/>
+      <c r="AM14" s="60"/>
+      <c r="AN14" s="60"/>
+      <c r="AO14" s="60"/>
+      <c r="AP14" s="60"/>
+      <c r="AQ14" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="AR14" s="50"/>
-      <c r="AS14" s="50"/>
-      <c r="AT14" s="51"/>
-      <c r="AU14" s="65"/>
-      <c r="AV14" s="66"/>
+      <c r="AR14" s="49"/>
+      <c r="AS14" s="49"/>
+      <c r="AT14" s="50"/>
+      <c r="AU14" s="51"/>
+      <c r="AV14" s="52"/>
     </row>
     <row r="15" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
@@ -4741,54 +4799,54 @@
       <c r="F15" s="62"/>
       <c r="G15" s="62"/>
       <c r="H15" s="62"/>
-      <c r="I15" s="49" t="s">
+      <c r="I15" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="48" t="s">
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="48"/>
-      <c r="U15" s="48"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="48"/>
-      <c r="X15" s="48"/>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="48"/>
-      <c r="AA15" s="48"/>
-      <c r="AB15" s="48"/>
-      <c r="AC15" s="64" t="s">
+      <c r="N15" s="61"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="61"/>
+      <c r="U15" s="61"/>
+      <c r="V15" s="61"/>
+      <c r="W15" s="61"/>
+      <c r="X15" s="61"/>
+      <c r="Y15" s="61"/>
+      <c r="Z15" s="61"/>
+      <c r="AA15" s="61"/>
+      <c r="AB15" s="61"/>
+      <c r="AC15" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="AD15" s="64"/>
-      <c r="AE15" s="64"/>
-      <c r="AF15" s="64"/>
-      <c r="AG15" s="64"/>
-      <c r="AH15" s="64"/>
-      <c r="AI15" s="64"/>
-      <c r="AJ15" s="64"/>
-      <c r="AK15" s="64"/>
-      <c r="AL15" s="64"/>
-      <c r="AM15" s="64"/>
-      <c r="AN15" s="64"/>
-      <c r="AO15" s="64"/>
-      <c r="AP15" s="64"/>
-      <c r="AQ15" s="49" t="s">
+      <c r="AD15" s="60"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="60"/>
+      <c r="AG15" s="60"/>
+      <c r="AH15" s="60"/>
+      <c r="AI15" s="60"/>
+      <c r="AJ15" s="60"/>
+      <c r="AK15" s="60"/>
+      <c r="AL15" s="60"/>
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="60"/>
+      <c r="AO15" s="60"/>
+      <c r="AP15" s="60"/>
+      <c r="AQ15" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="AR15" s="50"/>
-      <c r="AS15" s="50"/>
-      <c r="AT15" s="51"/>
-      <c r="AU15" s="65"/>
-      <c r="AV15" s="66"/>
+      <c r="AR15" s="49"/>
+      <c r="AS15" s="49"/>
+      <c r="AT15" s="50"/>
+      <c r="AU15" s="51"/>
+      <c r="AV15" s="52"/>
     </row>
     <row r="16" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
@@ -4802,54 +4860,54 @@
       <c r="F16" s="62"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
-      <c r="I16" s="49" t="s">
+      <c r="I16" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="48" t="s">
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="N16" s="48"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="48"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="48"/>
-      <c r="T16" s="48"/>
-      <c r="U16" s="48"/>
-      <c r="V16" s="48"/>
-      <c r="W16" s="48"/>
-      <c r="X16" s="48"/>
-      <c r="Y16" s="48"/>
-      <c r="Z16" s="48"/>
-      <c r="AA16" s="48"/>
-      <c r="AB16" s="48"/>
-      <c r="AC16" s="55" t="s">
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="61"/>
+      <c r="R16" s="61"/>
+      <c r="S16" s="61"/>
+      <c r="T16" s="61"/>
+      <c r="U16" s="61"/>
+      <c r="V16" s="61"/>
+      <c r="W16" s="61"/>
+      <c r="X16" s="61"/>
+      <c r="Y16" s="61"/>
+      <c r="Z16" s="61"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="AD16" s="56"/>
-      <c r="AE16" s="56"/>
-      <c r="AF16" s="56"/>
-      <c r="AG16" s="56"/>
-      <c r="AH16" s="56"/>
-      <c r="AI16" s="56"/>
-      <c r="AJ16" s="56"/>
-      <c r="AK16" s="56"/>
-      <c r="AL16" s="56"/>
-      <c r="AM16" s="56"/>
-      <c r="AN16" s="56"/>
-      <c r="AO16" s="56"/>
-      <c r="AP16" s="57"/>
-      <c r="AQ16" s="49" t="s">
+      <c r="AD16" s="57"/>
+      <c r="AE16" s="57"/>
+      <c r="AF16" s="57"/>
+      <c r="AG16" s="57"/>
+      <c r="AH16" s="57"/>
+      <c r="AI16" s="57"/>
+      <c r="AJ16" s="57"/>
+      <c r="AK16" s="57"/>
+      <c r="AL16" s="57"/>
+      <c r="AM16" s="57"/>
+      <c r="AN16" s="57"/>
+      <c r="AO16" s="57"/>
+      <c r="AP16" s="58"/>
+      <c r="AQ16" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="AR16" s="50"/>
-      <c r="AS16" s="50"/>
-      <c r="AT16" s="51"/>
-      <c r="AU16" s="65"/>
-      <c r="AV16" s="66"/>
+      <c r="AR16" s="49"/>
+      <c r="AS16" s="49"/>
+      <c r="AT16" s="50"/>
+      <c r="AU16" s="51"/>
+      <c r="AV16" s="52"/>
     </row>
     <row r="17" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -4863,54 +4921,54 @@
       <c r="F17" s="62"/>
       <c r="G17" s="62"/>
       <c r="H17" s="62"/>
-      <c r="I17" s="49" t="s">
+      <c r="I17" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="48" t="s">
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="48"/>
-      <c r="S17" s="48"/>
-      <c r="T17" s="48"/>
-      <c r="U17" s="48"/>
-      <c r="V17" s="48"/>
-      <c r="W17" s="48"/>
-      <c r="X17" s="48"/>
-      <c r="Y17" s="48"/>
-      <c r="Z17" s="48"/>
-      <c r="AA17" s="48"/>
-      <c r="AB17" s="48"/>
-      <c r="AC17" s="55" t="s">
+      <c r="N17" s="61"/>
+      <c r="O17" s="61"/>
+      <c r="P17" s="61"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="61"/>
+      <c r="S17" s="61"/>
+      <c r="T17" s="61"/>
+      <c r="U17" s="61"/>
+      <c r="V17" s="61"/>
+      <c r="W17" s="61"/>
+      <c r="X17" s="61"/>
+      <c r="Y17" s="61"/>
+      <c r="Z17" s="61"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="AD17" s="56"/>
-      <c r="AE17" s="56"/>
-      <c r="AF17" s="56"/>
-      <c r="AG17" s="56"/>
-      <c r="AH17" s="56"/>
-      <c r="AI17" s="56"/>
-      <c r="AJ17" s="56"/>
-      <c r="AK17" s="56"/>
-      <c r="AL17" s="56"/>
-      <c r="AM17" s="56"/>
-      <c r="AN17" s="56"/>
-      <c r="AO17" s="56"/>
-      <c r="AP17" s="57"/>
-      <c r="AQ17" s="49" t="s">
+      <c r="AD17" s="57"/>
+      <c r="AE17" s="57"/>
+      <c r="AF17" s="57"/>
+      <c r="AG17" s="57"/>
+      <c r="AH17" s="57"/>
+      <c r="AI17" s="57"/>
+      <c r="AJ17" s="57"/>
+      <c r="AK17" s="57"/>
+      <c r="AL17" s="57"/>
+      <c r="AM17" s="57"/>
+      <c r="AN17" s="57"/>
+      <c r="AO17" s="57"/>
+      <c r="AP17" s="58"/>
+      <c r="AQ17" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="AR17" s="50"/>
-      <c r="AS17" s="50"/>
-      <c r="AT17" s="51"/>
-      <c r="AU17" s="65"/>
-      <c r="AV17" s="66"/>
+      <c r="AR17" s="49"/>
+      <c r="AS17" s="49"/>
+      <c r="AT17" s="50"/>
+      <c r="AU17" s="51"/>
+      <c r="AV17" s="52"/>
     </row>
     <row r="18" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -4924,54 +4982,54 @@
       <c r="F18" s="62"/>
       <c r="G18" s="62"/>
       <c r="H18" s="62"/>
-      <c r="I18" s="49" t="s">
+      <c r="I18" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="48" t="s">
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="48"/>
-      <c r="U18" s="48"/>
-      <c r="V18" s="48"/>
-      <c r="W18" s="48"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="48"/>
-      <c r="Z18" s="48"/>
-      <c r="AA18" s="48"/>
-      <c r="AB18" s="48"/>
-      <c r="AC18" s="55" t="s">
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="61"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="AD18" s="56"/>
-      <c r="AE18" s="56"/>
-      <c r="AF18" s="56"/>
-      <c r="AG18" s="56"/>
-      <c r="AH18" s="56"/>
-      <c r="AI18" s="56"/>
-      <c r="AJ18" s="56"/>
-      <c r="AK18" s="56"/>
-      <c r="AL18" s="56"/>
-      <c r="AM18" s="56"/>
-      <c r="AN18" s="56"/>
-      <c r="AO18" s="56"/>
-      <c r="AP18" s="57"/>
-      <c r="AQ18" s="49" t="s">
+      <c r="AD18" s="57"/>
+      <c r="AE18" s="57"/>
+      <c r="AF18" s="57"/>
+      <c r="AG18" s="57"/>
+      <c r="AH18" s="57"/>
+      <c r="AI18" s="57"/>
+      <c r="AJ18" s="57"/>
+      <c r="AK18" s="57"/>
+      <c r="AL18" s="57"/>
+      <c r="AM18" s="57"/>
+      <c r="AN18" s="57"/>
+      <c r="AO18" s="57"/>
+      <c r="AP18" s="58"/>
+      <c r="AQ18" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AR18" s="50"/>
-      <c r="AS18" s="50"/>
-      <c r="AT18" s="51"/>
-      <c r="AU18" s="65"/>
-      <c r="AV18" s="66"/>
+      <c r="AR18" s="49"/>
+      <c r="AS18" s="49"/>
+      <c r="AT18" s="50"/>
+      <c r="AU18" s="51"/>
+      <c r="AV18" s="52"/>
     </row>
     <row r="19" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -4985,54 +5043,54 @@
       <c r="F19" s="62"/>
       <c r="G19" s="62"/>
       <c r="H19" s="62"/>
-      <c r="I19" s="49" t="s">
+      <c r="I19" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="48" t="s">
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="48"/>
-      <c r="S19" s="48"/>
-      <c r="T19" s="48"/>
-      <c r="U19" s="48"/>
-      <c r="V19" s="48"/>
-      <c r="W19" s="48"/>
-      <c r="X19" s="48"/>
-      <c r="Y19" s="48"/>
-      <c r="Z19" s="48"/>
-      <c r="AA19" s="48"/>
-      <c r="AB19" s="48"/>
-      <c r="AC19" s="55" t="s">
+      <c r="N19" s="61"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="61"/>
+      <c r="S19" s="61"/>
+      <c r="T19" s="61"/>
+      <c r="U19" s="61"/>
+      <c r="V19" s="61"/>
+      <c r="W19" s="61"/>
+      <c r="X19" s="61"/>
+      <c r="Y19" s="61"/>
+      <c r="Z19" s="61"/>
+      <c r="AA19" s="61"/>
+      <c r="AB19" s="61"/>
+      <c r="AC19" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="AD19" s="56"/>
-      <c r="AE19" s="56"/>
-      <c r="AF19" s="56"/>
-      <c r="AG19" s="56"/>
-      <c r="AH19" s="56"/>
-      <c r="AI19" s="56"/>
-      <c r="AJ19" s="56"/>
-      <c r="AK19" s="56"/>
-      <c r="AL19" s="56"/>
-      <c r="AM19" s="56"/>
-      <c r="AN19" s="56"/>
-      <c r="AO19" s="56"/>
-      <c r="AP19" s="57"/>
-      <c r="AQ19" s="49" t="s">
+      <c r="AD19" s="57"/>
+      <c r="AE19" s="57"/>
+      <c r="AF19" s="57"/>
+      <c r="AG19" s="57"/>
+      <c r="AH19" s="57"/>
+      <c r="AI19" s="57"/>
+      <c r="AJ19" s="57"/>
+      <c r="AK19" s="57"/>
+      <c r="AL19" s="57"/>
+      <c r="AM19" s="57"/>
+      <c r="AN19" s="57"/>
+      <c r="AO19" s="57"/>
+      <c r="AP19" s="58"/>
+      <c r="AQ19" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="AR19" s="50"/>
-      <c r="AS19" s="50"/>
-      <c r="AT19" s="51"/>
-      <c r="AU19" s="65"/>
-      <c r="AV19" s="66"/>
+      <c r="AR19" s="49"/>
+      <c r="AS19" s="49"/>
+      <c r="AT19" s="50"/>
+      <c r="AU19" s="51"/>
+      <c r="AV19" s="52"/>
     </row>
     <row r="20" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
@@ -5046,54 +5104,54 @@
       <c r="F20" s="62"/>
       <c r="G20" s="62"/>
       <c r="H20" s="62"/>
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="48" t="s">
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="48"/>
-      <c r="T20" s="48"/>
-      <c r="U20" s="48"/>
-      <c r="V20" s="48"/>
-      <c r="W20" s="48"/>
-      <c r="X20" s="48"/>
-      <c r="Y20" s="48"/>
-      <c r="Z20" s="48"/>
-      <c r="AA20" s="48"/>
-      <c r="AB20" s="48"/>
-      <c r="AC20" s="55" t="s">
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
+      <c r="P20" s="61"/>
+      <c r="Q20" s="61"/>
+      <c r="R20" s="61"/>
+      <c r="S20" s="61"/>
+      <c r="T20" s="61"/>
+      <c r="U20" s="61"/>
+      <c r="V20" s="61"/>
+      <c r="W20" s="61"/>
+      <c r="X20" s="61"/>
+      <c r="Y20" s="61"/>
+      <c r="Z20" s="61"/>
+      <c r="AA20" s="61"/>
+      <c r="AB20" s="61"/>
+      <c r="AC20" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="AD20" s="56"/>
-      <c r="AE20" s="56"/>
-      <c r="AF20" s="56"/>
-      <c r="AG20" s="56"/>
-      <c r="AH20" s="56"/>
-      <c r="AI20" s="56"/>
-      <c r="AJ20" s="56"/>
-      <c r="AK20" s="56"/>
-      <c r="AL20" s="56"/>
-      <c r="AM20" s="56"/>
-      <c r="AN20" s="56"/>
-      <c r="AO20" s="56"/>
-      <c r="AP20" s="57"/>
-      <c r="AQ20" s="49" t="s">
+      <c r="AD20" s="57"/>
+      <c r="AE20" s="57"/>
+      <c r="AF20" s="57"/>
+      <c r="AG20" s="57"/>
+      <c r="AH20" s="57"/>
+      <c r="AI20" s="57"/>
+      <c r="AJ20" s="57"/>
+      <c r="AK20" s="57"/>
+      <c r="AL20" s="57"/>
+      <c r="AM20" s="57"/>
+      <c r="AN20" s="57"/>
+      <c r="AO20" s="57"/>
+      <c r="AP20" s="58"/>
+      <c r="AQ20" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="AR20" s="50"/>
-      <c r="AS20" s="50"/>
-      <c r="AT20" s="51"/>
-      <c r="AU20" s="65"/>
-      <c r="AV20" s="66"/>
+      <c r="AR20" s="49"/>
+      <c r="AS20" s="49"/>
+      <c r="AT20" s="50"/>
+      <c r="AU20" s="51"/>
+      <c r="AV20" s="52"/>
     </row>
     <row r="21" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
@@ -5107,54 +5165,54 @@
       <c r="F21" s="62"/>
       <c r="G21" s="62"/>
       <c r="H21" s="62"/>
-      <c r="I21" s="49" t="s">
+      <c r="I21" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="48" t="s">
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="48"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="48"/>
-      <c r="X21" s="48"/>
-      <c r="Y21" s="48"/>
-      <c r="Z21" s="48"/>
-      <c r="AA21" s="48"/>
-      <c r="AB21" s="48"/>
-      <c r="AC21" s="55" t="s">
+      <c r="N21" s="61"/>
+      <c r="O21" s="61"/>
+      <c r="P21" s="61"/>
+      <c r="Q21" s="61"/>
+      <c r="R21" s="61"/>
+      <c r="S21" s="61"/>
+      <c r="T21" s="61"/>
+      <c r="U21" s="61"/>
+      <c r="V21" s="61"/>
+      <c r="W21" s="61"/>
+      <c r="X21" s="61"/>
+      <c r="Y21" s="61"/>
+      <c r="Z21" s="61"/>
+      <c r="AA21" s="61"/>
+      <c r="AB21" s="61"/>
+      <c r="AC21" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="AD21" s="56"/>
-      <c r="AE21" s="56"/>
-      <c r="AF21" s="56"/>
-      <c r="AG21" s="56"/>
-      <c r="AH21" s="56"/>
-      <c r="AI21" s="56"/>
-      <c r="AJ21" s="56"/>
-      <c r="AK21" s="56"/>
-      <c r="AL21" s="56"/>
-      <c r="AM21" s="56"/>
-      <c r="AN21" s="56"/>
-      <c r="AO21" s="56"/>
-      <c r="AP21" s="57"/>
-      <c r="AQ21" s="49" t="s">
+      <c r="AD21" s="57"/>
+      <c r="AE21" s="57"/>
+      <c r="AF21" s="57"/>
+      <c r="AG21" s="57"/>
+      <c r="AH21" s="57"/>
+      <c r="AI21" s="57"/>
+      <c r="AJ21" s="57"/>
+      <c r="AK21" s="57"/>
+      <c r="AL21" s="57"/>
+      <c r="AM21" s="57"/>
+      <c r="AN21" s="57"/>
+      <c r="AO21" s="57"/>
+      <c r="AP21" s="58"/>
+      <c r="AQ21" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="AR21" s="50"/>
-      <c r="AS21" s="50"/>
-      <c r="AT21" s="51"/>
-      <c r="AU21" s="65"/>
-      <c r="AV21" s="66"/>
+      <c r="AR21" s="49"/>
+      <c r="AS21" s="49"/>
+      <c r="AT21" s="50"/>
+      <c r="AU21" s="51"/>
+      <c r="AV21" s="52"/>
     </row>
     <row r="22" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
@@ -18831,76 +18889,18 @@
       <c r="AV300" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="103">
-    <mergeCell ref="AQ21:AT21"/>
-    <mergeCell ref="AU21:AV21"/>
-    <mergeCell ref="AQ5:AT5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AQ6:AT6"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AQ7:AT7"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="AQ8:AT8"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="AQ18:AT18"/>
-    <mergeCell ref="AU18:AV18"/>
-    <mergeCell ref="AQ19:AT19"/>
-    <mergeCell ref="AU19:AV19"/>
-    <mergeCell ref="AQ20:AT20"/>
-    <mergeCell ref="AU20:AV20"/>
-    <mergeCell ref="AQ15:AT15"/>
-    <mergeCell ref="AU15:AV15"/>
-    <mergeCell ref="AQ16:AT16"/>
-    <mergeCell ref="AU16:AV16"/>
-    <mergeCell ref="AQ17:AT17"/>
-    <mergeCell ref="AU17:AV17"/>
-    <mergeCell ref="AQ4:AT4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AQ11:AT11"/>
-    <mergeCell ref="AU11:AV11"/>
-    <mergeCell ref="AQ12:AT12"/>
-    <mergeCell ref="AU12:AV12"/>
-    <mergeCell ref="AQ13:AT13"/>
-    <mergeCell ref="AU13:AV13"/>
-    <mergeCell ref="AQ14:AT14"/>
-    <mergeCell ref="AU14:AV14"/>
-    <mergeCell ref="AQ9:AT9"/>
-    <mergeCell ref="AU9:AV9"/>
-    <mergeCell ref="AQ10:AT10"/>
-    <mergeCell ref="AU10:AV10"/>
-    <mergeCell ref="AC16:AP16"/>
-    <mergeCell ref="AC17:AP17"/>
-    <mergeCell ref="AC18:AP18"/>
-    <mergeCell ref="AC19:AP19"/>
-    <mergeCell ref="AC20:AP20"/>
-    <mergeCell ref="AC21:AP21"/>
-    <mergeCell ref="AC10:AP10"/>
-    <mergeCell ref="AC11:AP11"/>
-    <mergeCell ref="AC12:AP12"/>
-    <mergeCell ref="AC13:AP13"/>
-    <mergeCell ref="AC14:AP14"/>
-    <mergeCell ref="AC15:AP15"/>
-    <mergeCell ref="M20:AB20"/>
-    <mergeCell ref="M21:AB21"/>
-    <mergeCell ref="M14:AB14"/>
-    <mergeCell ref="M15:AB15"/>
-    <mergeCell ref="M16:AB16"/>
-    <mergeCell ref="M17:AB17"/>
-    <mergeCell ref="M18:AB18"/>
-    <mergeCell ref="M19:AB19"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="M12:AB12"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="M13:AB13"/>
-    <mergeCell ref="B14:H21"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I21:L21"/>
+  <mergeCells count="104">
+    <mergeCell ref="A3:AV3"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA2"/>
+    <mergeCell ref="AB1:AV2"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:V2"/>
     <mergeCell ref="M11:AB11"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="M7:AB7"/>
@@ -18925,16 +18925,75 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="M10:AB10"/>
     <mergeCell ref="I11:L11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA2"/>
-    <mergeCell ref="AB1:AV2"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:V2"/>
+    <mergeCell ref="B14:H21"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="M20:AB20"/>
+    <mergeCell ref="M21:AB21"/>
+    <mergeCell ref="M14:AB14"/>
+    <mergeCell ref="M15:AB15"/>
+    <mergeCell ref="M16:AB16"/>
+    <mergeCell ref="M17:AB17"/>
+    <mergeCell ref="M18:AB18"/>
+    <mergeCell ref="M19:AB19"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="M12:AB12"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="M13:AB13"/>
+    <mergeCell ref="AC16:AP16"/>
+    <mergeCell ref="AC17:AP17"/>
+    <mergeCell ref="AC18:AP18"/>
+    <mergeCell ref="AC19:AP19"/>
+    <mergeCell ref="AC20:AP20"/>
+    <mergeCell ref="AC21:AP21"/>
+    <mergeCell ref="AC10:AP10"/>
+    <mergeCell ref="AC11:AP11"/>
+    <mergeCell ref="AC12:AP12"/>
+    <mergeCell ref="AC13:AP13"/>
+    <mergeCell ref="AC14:AP14"/>
+    <mergeCell ref="AC15:AP15"/>
+    <mergeCell ref="AQ4:AT4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AQ11:AT11"/>
+    <mergeCell ref="AU11:AV11"/>
+    <mergeCell ref="AQ12:AT12"/>
+    <mergeCell ref="AU12:AV12"/>
+    <mergeCell ref="AQ13:AT13"/>
+    <mergeCell ref="AU13:AV13"/>
+    <mergeCell ref="AQ14:AT14"/>
+    <mergeCell ref="AU14:AV14"/>
+    <mergeCell ref="AQ9:AT9"/>
+    <mergeCell ref="AU9:AV9"/>
+    <mergeCell ref="AQ10:AT10"/>
+    <mergeCell ref="AU10:AV10"/>
+    <mergeCell ref="AQ21:AT21"/>
+    <mergeCell ref="AU21:AV21"/>
+    <mergeCell ref="AQ5:AT5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AQ6:AT6"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AQ7:AT7"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="AQ8:AT8"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="AQ18:AT18"/>
+    <mergeCell ref="AU18:AV18"/>
+    <mergeCell ref="AQ19:AT19"/>
+    <mergeCell ref="AU19:AV19"/>
+    <mergeCell ref="AQ20:AT20"/>
+    <mergeCell ref="AU20:AV20"/>
+    <mergeCell ref="AQ15:AT15"/>
+    <mergeCell ref="AU15:AV15"/>
+    <mergeCell ref="AQ16:AT16"/>
+    <mergeCell ref="AU16:AV16"/>
+    <mergeCell ref="AQ17:AT17"/>
+    <mergeCell ref="AU17:AV17"/>
   </mergeCells>
   <conditionalFormatting sqref="AU5:AV21">
     <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="FIXING">
@@ -19143,6 +19202,157 @@
   <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:48" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="29" t="str">
+        <f>ChucNang!M6</f>
+        <v>Quản lí thông tin cá nhân</v>
+      </c>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="31"/>
+    </row>
+    <row r="2" spans="1:48" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47">
+        <v>42371</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="47">
+        <v>42401</v>
+      </c>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="AB1:AV2"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:V2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AV2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -19185,8 +19395,8 @@
       <c r="Z1" s="36"/>
       <c r="AA1" s="37"/>
       <c r="AB1" s="29" t="str">
-        <f>ChucNang!M6</f>
-        <v>Quản lí thông tin cá nhân</v>
+        <f>ChucNang!M7</f>
+        <v>Quản lí danh mục hàng hóa</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="30"/>
@@ -19282,7 +19492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
@@ -19332,8 +19542,8 @@
       <c r="Z1" s="36"/>
       <c r="AA1" s="37"/>
       <c r="AB1" s="29" t="str">
-        <f>ChucNang!M7</f>
-        <v>Quản lí danh mục hàng hóa</v>
+        <f>ChucNang!M8</f>
+        <v>Quản lí hàng hóa</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="30"/>
@@ -19429,7 +19639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
@@ -19479,8 +19689,8 @@
       <c r="Z1" s="36"/>
       <c r="AA1" s="37"/>
       <c r="AB1" s="29" t="str">
-        <f>ChucNang!M8</f>
-        <v>Quản lí hàng hóa</v>
+        <f>ChucNang!M9</f>
+        <v>Quản lí thông tin User</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="30"/>
@@ -19576,7 +19786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
@@ -19626,8 +19836,8 @@
       <c r="Z1" s="36"/>
       <c r="AA1" s="37"/>
       <c r="AB1" s="29" t="str">
-        <f>ChucNang!M9</f>
-        <v>Quản lí thông tin User</v>
+        <f>ChucNang!M10</f>
+        <v>Quản lí Order (Đơn đặt hàng)</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="30"/>
@@ -19721,151 +19931,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="7" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:AV2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:48" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="29" t="str">
-        <f>ChucNang!M10</f>
-        <v>Quản lí Order (Đơn đặt hàng)</v>
-      </c>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
-      <c r="AO1" s="30"/>
-      <c r="AP1" s="30"/>
-      <c r="AQ1" s="30"/>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="31"/>
-    </row>
-    <row r="2" spans="1:48" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47">
-        <v>42371</v>
-      </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="34"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="AB1:AV2"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:V2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
#TM_NhanTV: Commit Document update
</commit_message>
<xml_diff>
--- a/01_Document/TM_Design_v1.0.xlsx
+++ b/01_Document/TM_Design_v1.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NTP\TimMart\01_Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Document\TimMartProject\TimMart\01_Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" tabRatio="880" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" tabRatio="880"/>
   </bookViews>
   <sheets>
     <sheet name="MoDau" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="104">
   <si>
     <t>Người tạo</t>
   </si>
@@ -822,6 +822,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,11 +837,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -846,14 +861,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -861,22 +873,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -884,7 +884,35 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1381,7 +1409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3397,11 +3425,290 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV21"/>
+  <dimension ref="A1:AV13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:48" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="31"/>
+    </row>
+    <row r="2" spans="1:48" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47">
+        <v>42371</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="47">
+        <v>42372</v>
+      </c>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="34"/>
+    </row>
+    <row r="3" spans="1:48" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" s="4"/>
+    </row>
+    <row r="5" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X8" s="6"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="P2:V2"/>
+    <mergeCell ref="AB1:AV2"/>
+    <mergeCell ref="W1:AA2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="L2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:AV2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3442,8 +3749,9 @@
       <c r="Y1" s="36"/>
       <c r="Z1" s="36"/>
       <c r="AA1" s="37"/>
-      <c r="AB1" s="29" t="s">
-        <v>5</v>
+      <c r="AB1" s="29" t="str">
+        <f>ChucNang!M21</f>
+        <v>Tồn kho</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="30"/>
@@ -3522,214 +3830,85 @@
       <c r="AU2" s="33"/>
       <c r="AV2" s="34"/>
     </row>
-    <row r="3" spans="1:48" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="X4" s="4"/>
-    </row>
-    <row r="5" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="6"/>
-      <c r="I6" s="5"/>
-      <c r="X6" s="6"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="X8" s="6"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="6"/>
-      <c r="I10" s="5"/>
-      <c r="X10" s="6"/>
-      <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="6"/>
-      <c r="I11" s="5"/>
-      <c r="X11" s="6"/>
-      <c r="AB11" s="3"/>
-    </row>
-    <row r="12" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X12" s="6"/>
-      <c r="AB12" s="3"/>
-    </row>
-    <row r="13" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="6"/>
-      <c r="I13" s="5"/>
-      <c r="X13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="X14" s="6"/>
-      <c r="AB14" s="3"/>
-    </row>
-    <row r="15" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="6"/>
-      <c r="I15" s="5"/>
-      <c r="X15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB15" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="6"/>
-      <c r="I16" s="5"/>
-      <c r="X16" s="6"/>
-      <c r="AB16" s="3"/>
-    </row>
-    <row r="17" spans="4:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="X17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB17" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="4:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="6"/>
-      <c r="I18" s="5"/>
-      <c r="X18" s="6"/>
-      <c r="AB18" s="3"/>
-    </row>
-    <row r="19" spans="4:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="X19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB19" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="4:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="6"/>
-      <c r="I20" s="5"/>
-      <c r="X20" s="6"/>
-      <c r="AB20" s="3"/>
-    </row>
-    <row r="21" spans="4:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="X21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB21" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB1:AV2"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:V2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:V1"/>
-    <mergeCell ref="P2:V2"/>
-    <mergeCell ref="AB1:AV2"/>
     <mergeCell ref="W1:AA2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="L2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="4" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AV300"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" style="9"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:48" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
@@ -3753,7 +3932,9 @@
       <c r="M1" s="42"/>
       <c r="N1" s="42"/>
       <c r="O1" s="43"/>
-      <c r="P1" s="26"/>
+      <c r="P1" s="26" t="s">
+        <v>6</v>
+      </c>
       <c r="Q1" s="27"/>
       <c r="R1" s="27"/>
       <c r="S1" s="27"/>
@@ -3767,9 +3948,8 @@
       <c r="Y1" s="36"/>
       <c r="Z1" s="36"/>
       <c r="AA1" s="37"/>
-      <c r="AB1" s="29" t="str">
-        <f>ChucNang!M21</f>
-        <v>Tồn kho</v>
+      <c r="AB1" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="30"/>
@@ -3814,7 +3994,9 @@
       <c r="M2" s="45"/>
       <c r="N2" s="45"/>
       <c r="O2" s="46"/>
-      <c r="P2" s="26"/>
+      <c r="P2" s="47">
+        <v>42372</v>
+      </c>
       <c r="Q2" s="27"/>
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
@@ -3848,881 +4030,671 @@
       <c r="AU2" s="33"/>
       <c r="AV2" s="34"/>
     </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="AB1:AV2"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:V2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV300"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:AV3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:48" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
-      <c r="AO1" s="30"/>
-      <c r="AP1" s="30"/>
-      <c r="AQ1" s="30"/>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="31"/>
-    </row>
-    <row r="2" spans="1:48" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47">
-        <v>42371</v>
-      </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="34"/>
-    </row>
     <row r="3" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
-      <c r="AK3" s="64"/>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-      <c r="AV3" s="64"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="48"/>
+      <c r="AJ3" s="48"/>
+      <c r="AK3" s="48"/>
+      <c r="AL3" s="48"/>
+      <c r="AM3" s="48"/>
+      <c r="AN3" s="48"/>
+      <c r="AO3" s="48"/>
+      <c r="AP3" s="48"/>
+      <c r="AQ3" s="48"/>
+      <c r="AR3" s="48"/>
+      <c r="AS3" s="48"/>
+      <c r="AT3" s="48"/>
+      <c r="AU3" s="48"/>
+      <c r="AV3" s="48"/>
     </row>
     <row r="4" spans="1:48" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="53" t="s">
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="53" t="s">
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="54"/>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="54"/>
-      <c r="AA4" s="54"/>
-      <c r="AB4" s="55"/>
-      <c r="AC4" s="53" t="s">
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="60"/>
+      <c r="AC4" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="AD4" s="54"/>
-      <c r="AE4" s="54"/>
-      <c r="AF4" s="54"/>
-      <c r="AG4" s="54"/>
-      <c r="AH4" s="54"/>
-      <c r="AI4" s="54"/>
-      <c r="AJ4" s="54"/>
-      <c r="AK4" s="54"/>
-      <c r="AL4" s="54"/>
-      <c r="AM4" s="54"/>
-      <c r="AN4" s="54"/>
-      <c r="AO4" s="54"/>
-      <c r="AP4" s="55"/>
-      <c r="AQ4" s="53" t="s">
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59"/>
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59"/>
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59"/>
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59"/>
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="60"/>
+      <c r="AQ4" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="AR4" s="54"/>
-      <c r="AS4" s="54"/>
-      <c r="AT4" s="55"/>
-      <c r="AU4" s="53" t="s">
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="59"/>
+      <c r="AT4" s="60"/>
+      <c r="AU4" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="AV4" s="55"/>
+      <c r="AV4" s="60"/>
     </row>
     <row r="5" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="48" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="63" t="s">
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="64"/>
-      <c r="Z5" s="64"/>
-      <c r="AA5" s="64"/>
-      <c r="AB5" s="65"/>
-      <c r="AC5" s="56" t="s">
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="AD5" s="57"/>
-      <c r="AE5" s="57"/>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="57"/>
-      <c r="AH5" s="57"/>
-      <c r="AI5" s="57"/>
-      <c r="AJ5" s="57"/>
-      <c r="AK5" s="57"/>
-      <c r="AL5" s="57"/>
-      <c r="AM5" s="57"/>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="57"/>
-      <c r="AP5" s="58"/>
-      <c r="AQ5" s="48" t="s">
+      <c r="AD5" s="56"/>
+      <c r="AE5" s="56"/>
+      <c r="AF5" s="56"/>
+      <c r="AG5" s="56"/>
+      <c r="AH5" s="56"/>
+      <c r="AI5" s="56"/>
+      <c r="AJ5" s="56"/>
+      <c r="AK5" s="56"/>
+      <c r="AL5" s="56"/>
+      <c r="AM5" s="56"/>
+      <c r="AN5" s="56"/>
+      <c r="AO5" s="56"/>
+      <c r="AP5" s="57"/>
+      <c r="AQ5" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AR5" s="49"/>
-      <c r="AS5" s="49"/>
-      <c r="AT5" s="50"/>
-      <c r="AU5" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="AV5" s="52"/>
+      <c r="AR5" s="51"/>
+      <c r="AS5" s="51"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="65"/>
+      <c r="AV5" s="66"/>
     </row>
     <row r="6" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <f>MAX($A5)+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="48" t="s">
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="63" t="s">
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="64"/>
-      <c r="S6" s="64"/>
-      <c r="T6" s="64"/>
-      <c r="U6" s="64"/>
-      <c r="V6" s="64"/>
-      <c r="W6" s="64"/>
-      <c r="X6" s="64"/>
-      <c r="Y6" s="64"/>
-      <c r="Z6" s="64"/>
-      <c r="AA6" s="64"/>
-      <c r="AB6" s="65"/>
-      <c r="AC6" s="56" t="s">
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="48"/>
+      <c r="AA6" s="48"/>
+      <c r="AB6" s="54"/>
+      <c r="AC6" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="AD6" s="57"/>
-      <c r="AE6" s="57"/>
-      <c r="AF6" s="57"/>
-      <c r="AG6" s="57"/>
-      <c r="AH6" s="57"/>
-      <c r="AI6" s="57"/>
-      <c r="AJ6" s="57"/>
-      <c r="AK6" s="57"/>
-      <c r="AL6" s="57"/>
-      <c r="AM6" s="57"/>
-      <c r="AN6" s="57"/>
-      <c r="AO6" s="57"/>
-      <c r="AP6" s="58"/>
-      <c r="AQ6" s="48" t="s">
+      <c r="AD6" s="56"/>
+      <c r="AE6" s="56"/>
+      <c r="AF6" s="56"/>
+      <c r="AG6" s="56"/>
+      <c r="AH6" s="56"/>
+      <c r="AI6" s="56"/>
+      <c r="AJ6" s="56"/>
+      <c r="AK6" s="56"/>
+      <c r="AL6" s="56"/>
+      <c r="AM6" s="56"/>
+      <c r="AN6" s="56"/>
+      <c r="AO6" s="56"/>
+      <c r="AP6" s="57"/>
+      <c r="AQ6" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="AR6" s="49"/>
-      <c r="AS6" s="49"/>
-      <c r="AT6" s="50"/>
-      <c r="AU6" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV6" s="52"/>
+      <c r="AR6" s="51"/>
+      <c r="AS6" s="51"/>
+      <c r="AT6" s="52"/>
+      <c r="AU6" s="65"/>
+      <c r="AV6" s="66"/>
     </row>
     <row r="7" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <f t="shared" ref="A7:A21" si="0">MAX($A6)+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="48" t="s">
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="63" t="s">
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="64"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="65"/>
-      <c r="AC7" s="56" t="s">
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+      <c r="AA7" s="48"/>
+      <c r="AB7" s="54"/>
+      <c r="AC7" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="AD7" s="57"/>
-      <c r="AE7" s="57"/>
-      <c r="AF7" s="57"/>
-      <c r="AG7" s="57"/>
-      <c r="AH7" s="57"/>
-      <c r="AI7" s="57"/>
-      <c r="AJ7" s="57"/>
-      <c r="AK7" s="57"/>
-      <c r="AL7" s="57"/>
-      <c r="AM7" s="57"/>
-      <c r="AN7" s="57"/>
-      <c r="AO7" s="57"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="48" t="s">
+      <c r="AD7" s="56"/>
+      <c r="AE7" s="56"/>
+      <c r="AF7" s="56"/>
+      <c r="AG7" s="56"/>
+      <c r="AH7" s="56"/>
+      <c r="AI7" s="56"/>
+      <c r="AJ7" s="56"/>
+      <c r="AK7" s="56"/>
+      <c r="AL7" s="56"/>
+      <c r="AM7" s="56"/>
+      <c r="AN7" s="56"/>
+      <c r="AO7" s="56"/>
+      <c r="AP7" s="57"/>
+      <c r="AQ7" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="AR7" s="49"/>
-      <c r="AS7" s="49"/>
-      <c r="AT7" s="50"/>
-      <c r="AU7" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="AV7" s="52"/>
+      <c r="AR7" s="51"/>
+      <c r="AS7" s="51"/>
+      <c r="AT7" s="52"/>
+      <c r="AU7" s="65"/>
+      <c r="AV7" s="66"/>
     </row>
     <row r="8" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="48" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="61" t="s">
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="61"/>
-      <c r="O8" s="61"/>
-      <c r="P8" s="61"/>
-      <c r="Q8" s="61"/>
-      <c r="R8" s="61"/>
-      <c r="S8" s="61"/>
-      <c r="T8" s="61"/>
-      <c r="U8" s="61"/>
-      <c r="V8" s="61"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="61"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="56" t="s">
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="49"/>
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="49"/>
+      <c r="AC8" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="AD8" s="57"/>
-      <c r="AE8" s="57"/>
-      <c r="AF8" s="57"/>
-      <c r="AG8" s="57"/>
-      <c r="AH8" s="57"/>
-      <c r="AI8" s="57"/>
-      <c r="AJ8" s="57"/>
-      <c r="AK8" s="57"/>
-      <c r="AL8" s="57"/>
-      <c r="AM8" s="57"/>
-      <c r="AN8" s="57"/>
-      <c r="AO8" s="57"/>
-      <c r="AP8" s="58"/>
-      <c r="AQ8" s="48" t="s">
+      <c r="AD8" s="56"/>
+      <c r="AE8" s="56"/>
+      <c r="AF8" s="56"/>
+      <c r="AG8" s="56"/>
+      <c r="AH8" s="56"/>
+      <c r="AI8" s="56"/>
+      <c r="AJ8" s="56"/>
+      <c r="AK8" s="56"/>
+      <c r="AL8" s="56"/>
+      <c r="AM8" s="56"/>
+      <c r="AN8" s="56"/>
+      <c r="AO8" s="56"/>
+      <c r="AP8" s="57"/>
+      <c r="AQ8" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="AR8" s="49"/>
-      <c r="AS8" s="49"/>
-      <c r="AT8" s="50"/>
-      <c r="AU8" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV8" s="52"/>
+      <c r="AR8" s="51"/>
+      <c r="AS8" s="51"/>
+      <c r="AT8" s="52"/>
+      <c r="AU8" s="65"/>
+      <c r="AV8" s="66"/>
     </row>
     <row r="9" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="48" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="61" t="s">
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="N9" s="61"/>
-      <c r="O9" s="61"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="61"/>
-      <c r="R9" s="61"/>
-      <c r="S9" s="61"/>
-      <c r="T9" s="61"/>
-      <c r="U9" s="61"/>
-      <c r="V9" s="61"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="61"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="56" t="s">
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="AD9" s="57"/>
-      <c r="AE9" s="57"/>
-      <c r="AF9" s="57"/>
-      <c r="AG9" s="57"/>
-      <c r="AH9" s="57"/>
-      <c r="AI9" s="57"/>
-      <c r="AJ9" s="57"/>
-      <c r="AK9" s="57"/>
-      <c r="AL9" s="57"/>
-      <c r="AM9" s="57"/>
-      <c r="AN9" s="57"/>
-      <c r="AO9" s="57"/>
-      <c r="AP9" s="58"/>
-      <c r="AQ9" s="48" t="s">
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="56"/>
+      <c r="AF9" s="56"/>
+      <c r="AG9" s="56"/>
+      <c r="AH9" s="56"/>
+      <c r="AI9" s="56"/>
+      <c r="AJ9" s="56"/>
+      <c r="AK9" s="56"/>
+      <c r="AL9" s="56"/>
+      <c r="AM9" s="56"/>
+      <c r="AN9" s="56"/>
+      <c r="AO9" s="56"/>
+      <c r="AP9" s="57"/>
+      <c r="AQ9" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AR9" s="49"/>
-      <c r="AS9" s="49"/>
-      <c r="AT9" s="50"/>
-      <c r="AU9" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="AV9" s="52"/>
+      <c r="AR9" s="51"/>
+      <c r="AS9" s="51"/>
+      <c r="AT9" s="52"/>
+      <c r="AU9" s="65"/>
+      <c r="AV9" s="66"/>
     </row>
     <row r="10" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="48" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="61" t="s">
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="61"/>
-      <c r="O10" s="61"/>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="61"/>
-      <c r="S10" s="61"/>
-      <c r="T10" s="61"/>
-      <c r="U10" s="61"/>
-      <c r="V10" s="61"/>
-      <c r="W10" s="61"/>
-      <c r="X10" s="61"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="61"/>
-      <c r="AA10" s="61"/>
-      <c r="AB10" s="61"/>
-      <c r="AC10" s="56" t="s">
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49"/>
+      <c r="X10" s="49"/>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AA10" s="49"/>
+      <c r="AB10" s="49"/>
+      <c r="AC10" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="AD10" s="57"/>
-      <c r="AE10" s="57"/>
-      <c r="AF10" s="57"/>
-      <c r="AG10" s="57"/>
-      <c r="AH10" s="57"/>
-      <c r="AI10" s="57"/>
-      <c r="AJ10" s="57"/>
-      <c r="AK10" s="57"/>
-      <c r="AL10" s="57"/>
-      <c r="AM10" s="57"/>
-      <c r="AN10" s="57"/>
-      <c r="AO10" s="57"/>
-      <c r="AP10" s="58"/>
-      <c r="AQ10" s="48" t="s">
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="56"/>
+      <c r="AF10" s="56"/>
+      <c r="AG10" s="56"/>
+      <c r="AH10" s="56"/>
+      <c r="AI10" s="56"/>
+      <c r="AJ10" s="56"/>
+      <c r="AK10" s="56"/>
+      <c r="AL10" s="56"/>
+      <c r="AM10" s="56"/>
+      <c r="AN10" s="56"/>
+      <c r="AO10" s="56"/>
+      <c r="AP10" s="57"/>
+      <c r="AQ10" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="AR10" s="49"/>
-      <c r="AS10" s="49"/>
-      <c r="AT10" s="50"/>
-      <c r="AU10" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV10" s="52"/>
+      <c r="AR10" s="51"/>
+      <c r="AS10" s="51"/>
+      <c r="AT10" s="52"/>
+      <c r="AU10" s="65"/>
+      <c r="AV10" s="66"/>
     </row>
     <row r="11" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="48" t="s">
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="61" t="s">
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="N11" s="61"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="61"/>
-      <c r="S11" s="61"/>
-      <c r="T11" s="61"/>
-      <c r="U11" s="61"/>
-      <c r="V11" s="61"/>
-      <c r="W11" s="61"/>
-      <c r="X11" s="61"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="61"/>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="61"/>
-      <c r="AC11" s="59" t="s">
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="49"/>
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="49"/>
+      <c r="AC11" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="AD11" s="59"/>
-      <c r="AE11" s="59"/>
-      <c r="AF11" s="59"/>
-      <c r="AG11" s="59"/>
-      <c r="AH11" s="59"/>
-      <c r="AI11" s="59"/>
-      <c r="AJ11" s="59"/>
-      <c r="AK11" s="59"/>
-      <c r="AL11" s="59"/>
-      <c r="AM11" s="59"/>
-      <c r="AN11" s="59"/>
-      <c r="AO11" s="59"/>
-      <c r="AP11" s="59"/>
-      <c r="AQ11" s="48" t="s">
+      <c r="AD11" s="63"/>
+      <c r="AE11" s="63"/>
+      <c r="AF11" s="63"/>
+      <c r="AG11" s="63"/>
+      <c r="AH11" s="63"/>
+      <c r="AI11" s="63"/>
+      <c r="AJ11" s="63"/>
+      <c r="AK11" s="63"/>
+      <c r="AL11" s="63"/>
+      <c r="AM11" s="63"/>
+      <c r="AN11" s="63"/>
+      <c r="AO11" s="63"/>
+      <c r="AP11" s="63"/>
+      <c r="AQ11" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="AR11" s="49"/>
-      <c r="AS11" s="49"/>
-      <c r="AT11" s="50"/>
-      <c r="AU11" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="AV11" s="52"/>
+      <c r="AR11" s="51"/>
+      <c r="AS11" s="51"/>
+      <c r="AT11" s="52"/>
+      <c r="AU11" s="65"/>
+      <c r="AV11" s="66"/>
     </row>
     <row r="12" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="48" t="s">
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="61" t="s">
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="61"/>
-      <c r="S12" s="61"/>
-      <c r="T12" s="61"/>
-      <c r="U12" s="61"/>
-      <c r="V12" s="61"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="61"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="61"/>
-      <c r="AC12" s="60" t="s">
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="60"/>
-      <c r="AH12" s="60"/>
-      <c r="AI12" s="60"/>
-      <c r="AJ12" s="60"/>
-      <c r="AK12" s="60"/>
-      <c r="AL12" s="60"/>
-      <c r="AM12" s="60"/>
-      <c r="AN12" s="60"/>
-      <c r="AO12" s="60"/>
-      <c r="AP12" s="60"/>
-      <c r="AQ12" s="48" t="s">
+      <c r="AD12" s="64"/>
+      <c r="AE12" s="64"/>
+      <c r="AF12" s="64"/>
+      <c r="AG12" s="64"/>
+      <c r="AH12" s="64"/>
+      <c r="AI12" s="64"/>
+      <c r="AJ12" s="64"/>
+      <c r="AK12" s="64"/>
+      <c r="AL12" s="64"/>
+      <c r="AM12" s="64"/>
+      <c r="AN12" s="64"/>
+      <c r="AO12" s="64"/>
+      <c r="AP12" s="64"/>
+      <c r="AQ12" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AR12" s="49"/>
-      <c r="AS12" s="49"/>
-      <c r="AT12" s="50"/>
-      <c r="AU12" s="51"/>
-      <c r="AV12" s="52"/>
+      <c r="AR12" s="51"/>
+      <c r="AS12" s="51"/>
+      <c r="AT12" s="52"/>
+      <c r="AU12" s="65"/>
+      <c r="AV12" s="66"/>
     </row>
     <row r="13" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="48" t="s">
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="61" t="s">
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="N13" s="61"/>
-      <c r="O13" s="61"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="61"/>
-      <c r="S13" s="61"/>
-      <c r="T13" s="61"/>
-      <c r="U13" s="61"/>
-      <c r="V13" s="61"/>
-      <c r="W13" s="61"/>
-      <c r="X13" s="61"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="61"/>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="61"/>
-      <c r="AC13" s="60" t="s">
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="49"/>
+      <c r="V13" s="49"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="49"/>
+      <c r="Y13" s="49"/>
+      <c r="Z13" s="49"/>
+      <c r="AA13" s="49"/>
+      <c r="AB13" s="49"/>
+      <c r="AC13" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
-      <c r="AH13" s="60"/>
-      <c r="AI13" s="60"/>
-      <c r="AJ13" s="60"/>
-      <c r="AK13" s="60"/>
-      <c r="AL13" s="60"/>
-      <c r="AM13" s="60"/>
-      <c r="AN13" s="60"/>
-      <c r="AO13" s="60"/>
-      <c r="AP13" s="60"/>
-      <c r="AQ13" s="48" t="s">
+      <c r="AD13" s="64"/>
+      <c r="AE13" s="64"/>
+      <c r="AF13" s="64"/>
+      <c r="AG13" s="64"/>
+      <c r="AH13" s="64"/>
+      <c r="AI13" s="64"/>
+      <c r="AJ13" s="64"/>
+      <c r="AK13" s="64"/>
+      <c r="AL13" s="64"/>
+      <c r="AM13" s="64"/>
+      <c r="AN13" s="64"/>
+      <c r="AO13" s="64"/>
+      <c r="AP13" s="64"/>
+      <c r="AQ13" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AR13" s="49"/>
-      <c r="AS13" s="49"/>
-      <c r="AT13" s="50"/>
-      <c r="AU13" s="51"/>
-      <c r="AV13" s="52"/>
+      <c r="AR13" s="51"/>
+      <c r="AS13" s="51"/>
+      <c r="AT13" s="52"/>
+      <c r="AU13" s="65"/>
+      <c r="AV13" s="66"/>
     </row>
     <row r="14" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -4738,54 +4710,54 @@
       <c r="F14" s="62"/>
       <c r="G14" s="62"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="48" t="s">
+      <c r="I14" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="61" t="s">
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="61"/>
-      <c r="S14" s="61"/>
-      <c r="T14" s="61"/>
-      <c r="U14" s="61"/>
-      <c r="V14" s="61"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="60" t="s">
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="49"/>
+      <c r="Z14" s="49"/>
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="49"/>
+      <c r="AC14" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="AD14" s="60"/>
-      <c r="AE14" s="60"/>
-      <c r="AF14" s="60"/>
-      <c r="AG14" s="60"/>
-      <c r="AH14" s="60"/>
-      <c r="AI14" s="60"/>
-      <c r="AJ14" s="60"/>
-      <c r="AK14" s="60"/>
-      <c r="AL14" s="60"/>
-      <c r="AM14" s="60"/>
-      <c r="AN14" s="60"/>
-      <c r="AO14" s="60"/>
-      <c r="AP14" s="60"/>
-      <c r="AQ14" s="48" t="s">
+      <c r="AD14" s="64"/>
+      <c r="AE14" s="64"/>
+      <c r="AF14" s="64"/>
+      <c r="AG14" s="64"/>
+      <c r="AH14" s="64"/>
+      <c r="AI14" s="64"/>
+      <c r="AJ14" s="64"/>
+      <c r="AK14" s="64"/>
+      <c r="AL14" s="64"/>
+      <c r="AM14" s="64"/>
+      <c r="AN14" s="64"/>
+      <c r="AO14" s="64"/>
+      <c r="AP14" s="64"/>
+      <c r="AQ14" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="AR14" s="49"/>
-      <c r="AS14" s="49"/>
-      <c r="AT14" s="50"/>
-      <c r="AU14" s="51"/>
-      <c r="AV14" s="52"/>
+      <c r="AR14" s="51"/>
+      <c r="AS14" s="51"/>
+      <c r="AT14" s="52"/>
+      <c r="AU14" s="65"/>
+      <c r="AV14" s="66"/>
     </row>
     <row r="15" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
@@ -4799,54 +4771,54 @@
       <c r="F15" s="62"/>
       <c r="G15" s="62"/>
       <c r="H15" s="62"/>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="61" t="s">
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="61"/>
-      <c r="S15" s="61"/>
-      <c r="T15" s="61"/>
-      <c r="U15" s="61"/>
-      <c r="V15" s="61"/>
-      <c r="W15" s="61"/>
-      <c r="X15" s="61"/>
-      <c r="Y15" s="61"/>
-      <c r="Z15" s="61"/>
-      <c r="AA15" s="61"/>
-      <c r="AB15" s="61"/>
-      <c r="AC15" s="60" t="s">
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="49"/>
+      <c r="Y15" s="49"/>
+      <c r="Z15" s="49"/>
+      <c r="AA15" s="49"/>
+      <c r="AB15" s="49"/>
+      <c r="AC15" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="AD15" s="60"/>
-      <c r="AE15" s="60"/>
-      <c r="AF15" s="60"/>
-      <c r="AG15" s="60"/>
-      <c r="AH15" s="60"/>
-      <c r="AI15" s="60"/>
-      <c r="AJ15" s="60"/>
-      <c r="AK15" s="60"/>
-      <c r="AL15" s="60"/>
-      <c r="AM15" s="60"/>
-      <c r="AN15" s="60"/>
-      <c r="AO15" s="60"/>
-      <c r="AP15" s="60"/>
-      <c r="AQ15" s="48" t="s">
+      <c r="AD15" s="64"/>
+      <c r="AE15" s="64"/>
+      <c r="AF15" s="64"/>
+      <c r="AG15" s="64"/>
+      <c r="AH15" s="64"/>
+      <c r="AI15" s="64"/>
+      <c r="AJ15" s="64"/>
+      <c r="AK15" s="64"/>
+      <c r="AL15" s="64"/>
+      <c r="AM15" s="64"/>
+      <c r="AN15" s="64"/>
+      <c r="AO15" s="64"/>
+      <c r="AP15" s="64"/>
+      <c r="AQ15" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="AR15" s="49"/>
-      <c r="AS15" s="49"/>
-      <c r="AT15" s="50"/>
-      <c r="AU15" s="51"/>
-      <c r="AV15" s="52"/>
+      <c r="AR15" s="51"/>
+      <c r="AS15" s="51"/>
+      <c r="AT15" s="52"/>
+      <c r="AU15" s="65"/>
+      <c r="AV15" s="66"/>
     </row>
     <row r="16" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
@@ -4860,54 +4832,54 @@
       <c r="F16" s="62"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="61" t="s">
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="61"/>
-      <c r="R16" s="61"/>
-      <c r="S16" s="61"/>
-      <c r="T16" s="61"/>
-      <c r="U16" s="61"/>
-      <c r="V16" s="61"/>
-      <c r="W16" s="61"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="56" t="s">
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="49"/>
+      <c r="V16" s="49"/>
+      <c r="W16" s="49"/>
+      <c r="X16" s="49"/>
+      <c r="Y16" s="49"/>
+      <c r="Z16" s="49"/>
+      <c r="AA16" s="49"/>
+      <c r="AB16" s="49"/>
+      <c r="AC16" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="AD16" s="57"/>
-      <c r="AE16" s="57"/>
-      <c r="AF16" s="57"/>
-      <c r="AG16" s="57"/>
-      <c r="AH16" s="57"/>
-      <c r="AI16" s="57"/>
-      <c r="AJ16" s="57"/>
-      <c r="AK16" s="57"/>
-      <c r="AL16" s="57"/>
-      <c r="AM16" s="57"/>
-      <c r="AN16" s="57"/>
-      <c r="AO16" s="57"/>
-      <c r="AP16" s="58"/>
-      <c r="AQ16" s="48" t="s">
+      <c r="AD16" s="56"/>
+      <c r="AE16" s="56"/>
+      <c r="AF16" s="56"/>
+      <c r="AG16" s="56"/>
+      <c r="AH16" s="56"/>
+      <c r="AI16" s="56"/>
+      <c r="AJ16" s="56"/>
+      <c r="AK16" s="56"/>
+      <c r="AL16" s="56"/>
+      <c r="AM16" s="56"/>
+      <c r="AN16" s="56"/>
+      <c r="AO16" s="56"/>
+      <c r="AP16" s="57"/>
+      <c r="AQ16" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="AR16" s="49"/>
-      <c r="AS16" s="49"/>
-      <c r="AT16" s="50"/>
-      <c r="AU16" s="51"/>
-      <c r="AV16" s="52"/>
+      <c r="AR16" s="51"/>
+      <c r="AS16" s="51"/>
+      <c r="AT16" s="52"/>
+      <c r="AU16" s="65"/>
+      <c r="AV16" s="66"/>
     </row>
     <row r="17" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -4921,54 +4893,54 @@
       <c r="F17" s="62"/>
       <c r="G17" s="62"/>
       <c r="H17" s="62"/>
-      <c r="I17" s="48" t="s">
+      <c r="I17" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="61" t="s">
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="61"/>
-      <c r="W17" s="61"/>
-      <c r="X17" s="61"/>
-      <c r="Y17" s="61"/>
-      <c r="Z17" s="61"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="56" t="s">
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="49"/>
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="49"/>
+      <c r="AA17" s="49"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="AD17" s="57"/>
-      <c r="AE17" s="57"/>
-      <c r="AF17" s="57"/>
-      <c r="AG17" s="57"/>
-      <c r="AH17" s="57"/>
-      <c r="AI17" s="57"/>
-      <c r="AJ17" s="57"/>
-      <c r="AK17" s="57"/>
-      <c r="AL17" s="57"/>
-      <c r="AM17" s="57"/>
-      <c r="AN17" s="57"/>
-      <c r="AO17" s="57"/>
-      <c r="AP17" s="58"/>
-      <c r="AQ17" s="48" t="s">
+      <c r="AD17" s="56"/>
+      <c r="AE17" s="56"/>
+      <c r="AF17" s="56"/>
+      <c r="AG17" s="56"/>
+      <c r="AH17" s="56"/>
+      <c r="AI17" s="56"/>
+      <c r="AJ17" s="56"/>
+      <c r="AK17" s="56"/>
+      <c r="AL17" s="56"/>
+      <c r="AM17" s="56"/>
+      <c r="AN17" s="56"/>
+      <c r="AO17" s="56"/>
+      <c r="AP17" s="57"/>
+      <c r="AQ17" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="AR17" s="49"/>
-      <c r="AS17" s="49"/>
-      <c r="AT17" s="50"/>
-      <c r="AU17" s="51"/>
-      <c r="AV17" s="52"/>
+      <c r="AR17" s="51"/>
+      <c r="AS17" s="51"/>
+      <c r="AT17" s="52"/>
+      <c r="AU17" s="65"/>
+      <c r="AV17" s="66"/>
     </row>
     <row r="18" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -4982,54 +4954,54 @@
       <c r="F18" s="62"/>
       <c r="G18" s="62"/>
       <c r="H18" s="62"/>
-      <c r="I18" s="48" t="s">
+      <c r="I18" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="61" t="s">
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="N18" s="61"/>
-      <c r="O18" s="61"/>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="61"/>
-      <c r="R18" s="61"/>
-      <c r="S18" s="61"/>
-      <c r="T18" s="61"/>
-      <c r="U18" s="61"/>
-      <c r="V18" s="61"/>
-      <c r="W18" s="61"/>
-      <c r="X18" s="61"/>
-      <c r="Y18" s="61"/>
-      <c r="Z18" s="61"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="56" t="s">
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="49"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="49"/>
+      <c r="AA18" s="49"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="AD18" s="57"/>
-      <c r="AE18" s="57"/>
-      <c r="AF18" s="57"/>
-      <c r="AG18" s="57"/>
-      <c r="AH18" s="57"/>
-      <c r="AI18" s="57"/>
-      <c r="AJ18" s="57"/>
-      <c r="AK18" s="57"/>
-      <c r="AL18" s="57"/>
-      <c r="AM18" s="57"/>
-      <c r="AN18" s="57"/>
-      <c r="AO18" s="57"/>
-      <c r="AP18" s="58"/>
-      <c r="AQ18" s="48" t="s">
+      <c r="AD18" s="56"/>
+      <c r="AE18" s="56"/>
+      <c r="AF18" s="56"/>
+      <c r="AG18" s="56"/>
+      <c r="AH18" s="56"/>
+      <c r="AI18" s="56"/>
+      <c r="AJ18" s="56"/>
+      <c r="AK18" s="56"/>
+      <c r="AL18" s="56"/>
+      <c r="AM18" s="56"/>
+      <c r="AN18" s="56"/>
+      <c r="AO18" s="56"/>
+      <c r="AP18" s="57"/>
+      <c r="AQ18" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AR18" s="49"/>
-      <c r="AS18" s="49"/>
-      <c r="AT18" s="50"/>
-      <c r="AU18" s="51"/>
-      <c r="AV18" s="52"/>
+      <c r="AR18" s="51"/>
+      <c r="AS18" s="51"/>
+      <c r="AT18" s="52"/>
+      <c r="AU18" s="65"/>
+      <c r="AV18" s="66"/>
     </row>
     <row r="19" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -5043,54 +5015,54 @@
       <c r="F19" s="62"/>
       <c r="G19" s="62"/>
       <c r="H19" s="62"/>
-      <c r="I19" s="48" t="s">
+      <c r="I19" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="61" t="s">
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="61"/>
-      <c r="S19" s="61"/>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="61"/>
-      <c r="W19" s="61"/>
-      <c r="X19" s="61"/>
-      <c r="Y19" s="61"/>
-      <c r="Z19" s="61"/>
-      <c r="AA19" s="61"/>
-      <c r="AB19" s="61"/>
-      <c r="AC19" s="56" t="s">
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="49"/>
+      <c r="W19" s="49"/>
+      <c r="X19" s="49"/>
+      <c r="Y19" s="49"/>
+      <c r="Z19" s="49"/>
+      <c r="AA19" s="49"/>
+      <c r="AB19" s="49"/>
+      <c r="AC19" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="AD19" s="57"/>
-      <c r="AE19" s="57"/>
-      <c r="AF19" s="57"/>
-      <c r="AG19" s="57"/>
-      <c r="AH19" s="57"/>
-      <c r="AI19" s="57"/>
-      <c r="AJ19" s="57"/>
-      <c r="AK19" s="57"/>
-      <c r="AL19" s="57"/>
-      <c r="AM19" s="57"/>
-      <c r="AN19" s="57"/>
-      <c r="AO19" s="57"/>
-      <c r="AP19" s="58"/>
-      <c r="AQ19" s="48" t="s">
+      <c r="AD19" s="56"/>
+      <c r="AE19" s="56"/>
+      <c r="AF19" s="56"/>
+      <c r="AG19" s="56"/>
+      <c r="AH19" s="56"/>
+      <c r="AI19" s="56"/>
+      <c r="AJ19" s="56"/>
+      <c r="AK19" s="56"/>
+      <c r="AL19" s="56"/>
+      <c r="AM19" s="56"/>
+      <c r="AN19" s="56"/>
+      <c r="AO19" s="56"/>
+      <c r="AP19" s="57"/>
+      <c r="AQ19" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="AR19" s="49"/>
-      <c r="AS19" s="49"/>
-      <c r="AT19" s="50"/>
-      <c r="AU19" s="51"/>
-      <c r="AV19" s="52"/>
+      <c r="AR19" s="51"/>
+      <c r="AS19" s="51"/>
+      <c r="AT19" s="52"/>
+      <c r="AU19" s="65"/>
+      <c r="AV19" s="66"/>
     </row>
     <row r="20" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
@@ -5104,54 +5076,54 @@
       <c r="F20" s="62"/>
       <c r="G20" s="62"/>
       <c r="H20" s="62"/>
-      <c r="I20" s="48" t="s">
+      <c r="I20" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="61" t="s">
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="N20" s="61"/>
-      <c r="O20" s="61"/>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="61"/>
-      <c r="R20" s="61"/>
-      <c r="S20" s="61"/>
-      <c r="T20" s="61"/>
-      <c r="U20" s="61"/>
-      <c r="V20" s="61"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
-      <c r="Y20" s="61"/>
-      <c r="Z20" s="61"/>
-      <c r="AA20" s="61"/>
-      <c r="AB20" s="61"/>
-      <c r="AC20" s="56" t="s">
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="49"/>
+      <c r="W20" s="49"/>
+      <c r="X20" s="49"/>
+      <c r="Y20" s="49"/>
+      <c r="Z20" s="49"/>
+      <c r="AA20" s="49"/>
+      <c r="AB20" s="49"/>
+      <c r="AC20" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="AD20" s="57"/>
-      <c r="AE20" s="57"/>
-      <c r="AF20" s="57"/>
-      <c r="AG20" s="57"/>
-      <c r="AH20" s="57"/>
-      <c r="AI20" s="57"/>
-      <c r="AJ20" s="57"/>
-      <c r="AK20" s="57"/>
-      <c r="AL20" s="57"/>
-      <c r="AM20" s="57"/>
-      <c r="AN20" s="57"/>
-      <c r="AO20" s="57"/>
-      <c r="AP20" s="58"/>
-      <c r="AQ20" s="48" t="s">
+      <c r="AD20" s="56"/>
+      <c r="AE20" s="56"/>
+      <c r="AF20" s="56"/>
+      <c r="AG20" s="56"/>
+      <c r="AH20" s="56"/>
+      <c r="AI20" s="56"/>
+      <c r="AJ20" s="56"/>
+      <c r="AK20" s="56"/>
+      <c r="AL20" s="56"/>
+      <c r="AM20" s="56"/>
+      <c r="AN20" s="56"/>
+      <c r="AO20" s="56"/>
+      <c r="AP20" s="57"/>
+      <c r="AQ20" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="AR20" s="49"/>
-      <c r="AS20" s="49"/>
-      <c r="AT20" s="50"/>
-      <c r="AU20" s="51"/>
-      <c r="AV20" s="52"/>
+      <c r="AR20" s="51"/>
+      <c r="AS20" s="51"/>
+      <c r="AT20" s="52"/>
+      <c r="AU20" s="65"/>
+      <c r="AV20" s="66"/>
     </row>
     <row r="21" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
@@ -5165,54 +5137,54 @@
       <c r="F21" s="62"/>
       <c r="G21" s="62"/>
       <c r="H21" s="62"/>
-      <c r="I21" s="48" t="s">
+      <c r="I21" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="61" t="s">
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="61"/>
-      <c r="O21" s="61"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="61"/>
-      <c r="R21" s="61"/>
-      <c r="S21" s="61"/>
-      <c r="T21" s="61"/>
-      <c r="U21" s="61"/>
-      <c r="V21" s="61"/>
-      <c r="W21" s="61"/>
-      <c r="X21" s="61"/>
-      <c r="Y21" s="61"/>
-      <c r="Z21" s="61"/>
-      <c r="AA21" s="61"/>
-      <c r="AB21" s="61"/>
-      <c r="AC21" s="56" t="s">
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="49"/>
+      <c r="V21" s="49"/>
+      <c r="W21" s="49"/>
+      <c r="X21" s="49"/>
+      <c r="Y21" s="49"/>
+      <c r="Z21" s="49"/>
+      <c r="AA21" s="49"/>
+      <c r="AB21" s="49"/>
+      <c r="AC21" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="AD21" s="57"/>
-      <c r="AE21" s="57"/>
-      <c r="AF21" s="57"/>
-      <c r="AG21" s="57"/>
-      <c r="AH21" s="57"/>
-      <c r="AI21" s="57"/>
-      <c r="AJ21" s="57"/>
-      <c r="AK21" s="57"/>
-      <c r="AL21" s="57"/>
-      <c r="AM21" s="57"/>
-      <c r="AN21" s="57"/>
-      <c r="AO21" s="57"/>
-      <c r="AP21" s="58"/>
-      <c r="AQ21" s="48" t="s">
+      <c r="AD21" s="56"/>
+      <c r="AE21" s="56"/>
+      <c r="AF21" s="56"/>
+      <c r="AG21" s="56"/>
+      <c r="AH21" s="56"/>
+      <c r="AI21" s="56"/>
+      <c r="AJ21" s="56"/>
+      <c r="AK21" s="56"/>
+      <c r="AL21" s="56"/>
+      <c r="AM21" s="56"/>
+      <c r="AN21" s="56"/>
+      <c r="AO21" s="56"/>
+      <c r="AP21" s="57"/>
+      <c r="AQ21" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="AR21" s="49"/>
-      <c r="AS21" s="49"/>
-      <c r="AT21" s="50"/>
-      <c r="AU21" s="51"/>
-      <c r="AV21" s="52"/>
+      <c r="AR21" s="51"/>
+      <c r="AS21" s="51"/>
+      <c r="AT21" s="52"/>
+      <c r="AU21" s="65"/>
+      <c r="AV21" s="66"/>
     </row>
     <row r="22" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
@@ -18890,17 +18862,75 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A3:AV3"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA2"/>
-    <mergeCell ref="AB1:AV2"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:V2"/>
+    <mergeCell ref="AQ21:AT21"/>
+    <mergeCell ref="AU21:AV21"/>
+    <mergeCell ref="AQ5:AT5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AQ6:AT6"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AQ7:AT7"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="AQ8:AT8"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="AQ18:AT18"/>
+    <mergeCell ref="AU18:AV18"/>
+    <mergeCell ref="AQ19:AT19"/>
+    <mergeCell ref="AU19:AV19"/>
+    <mergeCell ref="AQ20:AT20"/>
+    <mergeCell ref="AU20:AV20"/>
+    <mergeCell ref="AQ15:AT15"/>
+    <mergeCell ref="AU15:AV15"/>
+    <mergeCell ref="AQ16:AT16"/>
+    <mergeCell ref="AU16:AV16"/>
+    <mergeCell ref="AQ17:AT17"/>
+    <mergeCell ref="AU17:AV17"/>
+    <mergeCell ref="AQ4:AT4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AQ11:AT11"/>
+    <mergeCell ref="AU11:AV11"/>
+    <mergeCell ref="AQ12:AT12"/>
+    <mergeCell ref="AU12:AV12"/>
+    <mergeCell ref="AQ13:AT13"/>
+    <mergeCell ref="AU13:AV13"/>
+    <mergeCell ref="AQ14:AT14"/>
+    <mergeCell ref="AU14:AV14"/>
+    <mergeCell ref="AQ9:AT9"/>
+    <mergeCell ref="AU9:AV9"/>
+    <mergeCell ref="AQ10:AT10"/>
+    <mergeCell ref="AU10:AV10"/>
+    <mergeCell ref="AC16:AP16"/>
+    <mergeCell ref="AC17:AP17"/>
+    <mergeCell ref="AC18:AP18"/>
+    <mergeCell ref="AC19:AP19"/>
+    <mergeCell ref="AC20:AP20"/>
+    <mergeCell ref="AC21:AP21"/>
+    <mergeCell ref="AC10:AP10"/>
+    <mergeCell ref="AC11:AP11"/>
+    <mergeCell ref="AC12:AP12"/>
+    <mergeCell ref="AC13:AP13"/>
+    <mergeCell ref="AC14:AP14"/>
+    <mergeCell ref="AC15:AP15"/>
+    <mergeCell ref="M20:AB20"/>
+    <mergeCell ref="M21:AB21"/>
+    <mergeCell ref="M14:AB14"/>
+    <mergeCell ref="M15:AB15"/>
+    <mergeCell ref="M16:AB16"/>
+    <mergeCell ref="M17:AB17"/>
+    <mergeCell ref="M18:AB18"/>
+    <mergeCell ref="M19:AB19"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="M12:AB12"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="M13:AB13"/>
+    <mergeCell ref="B14:H21"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
     <mergeCell ref="M11:AB11"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="M7:AB7"/>
@@ -18925,92 +18955,34 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="M10:AB10"/>
     <mergeCell ref="I11:L11"/>
-    <mergeCell ref="B14:H21"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="M20:AB20"/>
-    <mergeCell ref="M21:AB21"/>
-    <mergeCell ref="M14:AB14"/>
-    <mergeCell ref="M15:AB15"/>
-    <mergeCell ref="M16:AB16"/>
-    <mergeCell ref="M17:AB17"/>
-    <mergeCell ref="M18:AB18"/>
-    <mergeCell ref="M19:AB19"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="M12:AB12"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="M13:AB13"/>
-    <mergeCell ref="AC16:AP16"/>
-    <mergeCell ref="AC17:AP17"/>
-    <mergeCell ref="AC18:AP18"/>
-    <mergeCell ref="AC19:AP19"/>
-    <mergeCell ref="AC20:AP20"/>
-    <mergeCell ref="AC21:AP21"/>
-    <mergeCell ref="AC10:AP10"/>
-    <mergeCell ref="AC11:AP11"/>
-    <mergeCell ref="AC12:AP12"/>
-    <mergeCell ref="AC13:AP13"/>
-    <mergeCell ref="AC14:AP14"/>
-    <mergeCell ref="AC15:AP15"/>
-    <mergeCell ref="AQ4:AT4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AQ11:AT11"/>
-    <mergeCell ref="AU11:AV11"/>
-    <mergeCell ref="AQ12:AT12"/>
-    <mergeCell ref="AU12:AV12"/>
-    <mergeCell ref="AQ13:AT13"/>
-    <mergeCell ref="AU13:AV13"/>
-    <mergeCell ref="AQ14:AT14"/>
-    <mergeCell ref="AU14:AV14"/>
-    <mergeCell ref="AQ9:AT9"/>
-    <mergeCell ref="AU9:AV9"/>
-    <mergeCell ref="AQ10:AT10"/>
-    <mergeCell ref="AU10:AV10"/>
-    <mergeCell ref="AQ21:AT21"/>
-    <mergeCell ref="AU21:AV21"/>
-    <mergeCell ref="AQ5:AT5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AQ6:AT6"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AQ7:AT7"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="AQ8:AT8"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="AQ18:AT18"/>
-    <mergeCell ref="AU18:AV18"/>
-    <mergeCell ref="AQ19:AT19"/>
-    <mergeCell ref="AU19:AV19"/>
-    <mergeCell ref="AQ20:AT20"/>
-    <mergeCell ref="AU20:AV20"/>
-    <mergeCell ref="AQ15:AT15"/>
-    <mergeCell ref="AU15:AV15"/>
-    <mergeCell ref="AQ16:AT16"/>
-    <mergeCell ref="AU16:AV16"/>
-    <mergeCell ref="AQ17:AT17"/>
-    <mergeCell ref="AU17:AV17"/>
+    <mergeCell ref="A3:AV3"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA2"/>
+    <mergeCell ref="AB1:AV2"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:V2"/>
   </mergeCells>
   <conditionalFormatting sqref="AU5:AV21">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="FIXING">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="FIXING">
       <formula>NOT(ISERROR(SEARCH("FIXING",AU5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH("BUG",AU5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",AU5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="10" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",AU5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU6:AV11">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="CODING">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="CODING">
       <formula>NOT(ISERROR(SEARCH("CODING",AU6)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>